<commit_message>
Add functionality now works
</commit_message>
<xml_diff>
--- a/data/inv.xlsx
+++ b/data/inv.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colton\HanaHou-INV\Inventory Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colton\SchoolProjects\CS453Projects\Final_Project\invy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FEC5CD-7E2F-4E48-9257-18F636369D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A370FB-698B-4EC8-8087-049B2025E4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02C0110B-5398-42D1-8FE1-0AEDAF00B9A1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02C0110B-5398-42D1-8FE1-0AEDAF00B9A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="590">
   <si>
     <t>Category</t>
   </si>
@@ -1798,6 +1798,12 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Poshmark URL</t>
+  </si>
+  <si>
+    <t>eBay URL</t>
   </si>
 </sst>
 </file>
@@ -1860,8 +1866,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{32458EFB-F94E-41BB-981D-825211C69C1B}" name="Table1" displayName="Table1" ref="A1:G374" totalsRowShown="0">
-  <autoFilter ref="A1:G374" xr:uid="{DC4E9A75-7651-4542-A646-5FE3CC6C4848}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{32458EFB-F94E-41BB-981D-825211C69C1B}" name="Table1" displayName="Table1" ref="A1:I374" totalsRowShown="0">
+  <autoFilter ref="A1:I374" xr:uid="{DC4E9A75-7651-4542-A646-5FE3CC6C4848}">
     <filterColumn colId="0">
       <filters>
         <filter val="Free People"/>
@@ -1871,7 +1877,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A38:G310">
     <sortCondition ref="F1:F374"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="9">
     <tableColumn id="2" xr3:uid="{BF3102F1-8340-479F-9F11-6C2BFEDE1DED}" name="Brand"/>
     <tableColumn id="1" xr3:uid="{3F8E9FAF-848B-4F42-BF7A-3F87B4DA9D64}" name="Category"/>
     <tableColumn id="3" xr3:uid="{E810883A-48FC-4706-8882-CB46C28193B3}" name="Subcategory"/>
@@ -1879,6 +1885,8 @@
     <tableColumn id="6" xr3:uid="{BDB03993-338D-4F2C-8453-E7015130C2D4}" name="Box Num"/>
     <tableColumn id="9" xr3:uid="{D08ADF3D-1B64-425F-A454-78EB7A49B9D1}" name="Number"/>
     <tableColumn id="7" xr3:uid="{DA4DB2D5-2C49-4EC6-AC6E-EBFCC7B2210D}" name="Style #"/>
+    <tableColumn id="5" xr3:uid="{E4531C6D-A0B5-4130-8250-FEC3E017FC52}" name="Poshmark URL"/>
+    <tableColumn id="8" xr3:uid="{E1F80C93-52B6-42CE-9F50-A7F5288F8B6F}" name="eBay URL"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2181,10 +2189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F007AC33-14E3-4845-B2C2-45DEBE8D7120}">
-  <dimension ref="A1:G374"/>
+  <dimension ref="A1:I374"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J132" sqref="J132"/>
+      <selection activeCell="L138" sqref="L132:L138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,10 +2204,11 @@
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2221,8 +2230,14 @@
       <c r="G1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>588</v>
+      </c>
+      <c r="I1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2239,7 +2254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>239</v>
       </c>
@@ -2259,7 +2274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>241</v>
       </c>
@@ -2276,7 +2291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>243</v>
       </c>
@@ -2296,7 +2311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -2313,7 +2328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>246</v>
       </c>
@@ -2333,7 +2348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>167</v>
       </c>
@@ -2350,7 +2365,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>249</v>
       </c>
@@ -2370,7 +2385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -2390,7 +2405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>254</v>
       </c>
@@ -2410,7 +2425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>255</v>
       </c>
@@ -2427,7 +2442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>257</v>
       </c>
@@ -2447,7 +2462,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>243</v>
       </c>
@@ -2467,7 +2482,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>260</v>
       </c>
@@ -2487,7 +2502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>243</v>
       </c>

</xml_diff>